<commit_message>
setup project + documentation added
</commit_message>
<xml_diff>
--- a/news_OutPutFile.xlsx
+++ b/news_OutPutFile.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
   </sheets>
   <definedNames>
-    <definedName name="Sheet1">'Sheet1'!$A$1:$I$4</definedName>
+    <definedName name="Sheet1">'Sheet1'!$A$1:$I$49</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -343,7 +343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -474,6 +474,1106 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>9/17/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>9/14/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>9/20/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>9/19/2018 3:24:41 PM</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Alibaba steps up push into chipmaking and quantum computers</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>Chinese tech group aims to bring its first AI chips to market next year</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t>China’s Alibaba is ramping up its push into leading-edge technologies, developing superfast quantum computers and</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/10d86136-bbe8-11e8-94b2-17176fbf93f5</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>12/17/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>12/14/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>12/20/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>1/8/2019 5:15:26 AM</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>IBM unveils first standalone quantum computer</t>
+        </is>
+      </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>Powerful new system could eventually leave today’s machines in the dust</t>
+        </is>
+      </c>
+      <c r="H8" s="0" t="inlineStr">
+        <is>
+          <t>This is one computer you will not be able to buy after the Consumer Electronics Show. IBM has built the first</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/f0d63c74-12c6-11e9-a581-4ff78404524e</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>Nike Inc</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>6/12/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>6/9/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>6/15/2017 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>6/14/2017 5:27:44 PM</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>Brussels probes merchandise ranges over potential ‘geo-blocking’</t>
+        </is>
+      </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>Antitrust authorities to look at sales practices at Nike, Universal Studios and Sanrio</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t>The companies behind Barcelona football shirts and the Minions and Hello Kitty ranges of merchandise are being</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/76a888d8-50ff-11e7-bfb8-997009366969</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>Nike Inc</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>9/17/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>9/14/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>9/20/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>9/13/2018 10:32:51 AM</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Nike, Kaepernick and the power of voting with the wallet</t>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>Why social justice is good for business</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t>Why did I find myself in Nike’s multistorey flagship store in New York last weekend? Was it a) because I had just seen</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/2f40b976-b688-11e8-b3ef-799c8613f4a1</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>Nike Inc</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>4/15/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>4/12/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>4/18/2019 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>Boeing Co</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>7/24/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>7/21/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>7/27/2017 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>7/26/2017 6:13:28 PM</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>Boeing results propel shares to all-time highs</t>
+        </is>
+      </c>
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t>US aerospace group delivers significantly better than expected performance in Q2</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t>Boeing shares leapt to an all-time high after the US aerospace and defence group delivered a significantly better than</t>
+        </is>
+      </c>
+      <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/681f87f6-7221-11e7-aca6-c6bd07df1a3c</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>Boeing Co</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>2/19/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>2/16/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>2/22/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>2/27/2018 11:17:03 AM</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>Safran plays down hopes for stepped up aircraft production</t>
+        </is>
+      </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>Supplier cool on push by Boeing and Airbus for faster deliveries of single-aisle jets</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t>Safran, the French jet engine maker, has poured cold water on a push by Boeing and Airbus to accelerate production of</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/0b7033fa-1b92-11e8-aaca-4574d7dabfb6</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>Procter &amp; Gamble Co</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>5/8/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>5/5/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>5/11/2017 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>5/10/2017 5:57:59 PM</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>Coty sales rebound in first sign of turnround</t>
+        </is>
+      </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>US cosmetics group is banking on reviving brands bought from P&amp;G</t>
+        </is>
+      </c>
+      <c r="H19" s="0" t="inlineStr">
+        <is>
+          <t>Sales growth at Coty bounced back in the quarter to the end of March as the US cosmetics group showed the first signs</t>
+        </is>
+      </c>
+      <c r="I19" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/d7d704d8-359b-11e7-99bd-13beb0903fa3</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>Procter &amp; Gamble Co</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>4/30/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>4/27/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>5/3/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>5/2/2018 4:00:43 AM</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>Scepticism over ‘value’ comeback despite energy surge</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Investment strategy gains are over-reliant on one sector, reflecting little broader shift</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>Energy shares were the top US market performers over the past month but the move has not been enough to renew faith</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/d3d4cacc-4cb1-11e8-97e4-13afc22d86d4</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>American Express Company</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>1/1/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>12/29/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>1/4/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="23">
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>1/19/2018 5:15:26 AM</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>US banks’ mission to boost investor payouts sparks concern</t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>Moves to trim capital cushions while boosting payouts is worrying, say some observers</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t>Michael Corbat was quite clear. The $22bn charge that Citigroup just took due to the overhaul of US tax laws would not</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/d9f84f8a-fcae-11e7-9b32-d7d59aace167</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="24">
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>1/18/2018 10:00:00 PM</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>American Express suspends buybacks after tax hit</t>
+        </is>
+      </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>Credit card issuer posts quarterly loss</t>
+        </is>
+      </c>
+      <c r="H24" s="0" t="inlineStr">
+        <is>
+          <t>American Express on Thursday said it plans to suspend its share buyback programme as a result of the tax reform that</t>
+        </is>
+      </c>
+      <c r="I24" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/a1b63d42-fc88-11e7-9b32-d7d59aace167</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>American Express Company</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>12/17/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>12/14/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>12/20/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>Visa Inc</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>9/24/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>9/21/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>9/27/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="27">
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>9/23/2018 11:39:07 AM</t>
+        </is>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>Legal settlement brings card issuers scant relief</t>
+        </is>
+      </c>
+      <c r="G27" s="0" t="inlineStr">
+        <is>
+          <t>Main battle over rules imposed on merchants begins next year</t>
+        </is>
+      </c>
+      <c r="H27" s="0" t="inlineStr">
+        <is>
+          <t>As president of a family business – a chain of 34 gas stations and convenience stores in Northern California, under the</t>
+        </is>
+      </c>
+      <c r="I27" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/f4c6dbf8-bde0-11e8-94b2-17176fbf93f5</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="28">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>Coca-Cola Co</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>1/22/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>1/19/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>1/25/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="29">
+      <c r="E29" s="0" t="inlineStr">
+        <is>
+          <t>1/22/2018 11:50:44 AM</t>
+        </is>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>Consumer goods groups join war on plastic</t>
+        </is>
+      </c>
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t>Big names from Coke to Unilever address concerns as customers and governments urge action</t>
+        </is>
+      </c>
+      <c r="H29" s="0" t="inlineStr">
+        <is>
+          <t>When Coca-Cola announced ambitious new targets for package recycling last week, the decision was not solely driven by</t>
+        </is>
+      </c>
+      <c r="I29" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/61629224-fc9f-11e7-9b32-d7d59aace167</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="30">
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t>1/19/2018 5:42:12 PM</t>
+        </is>
+      </c>
+      <c r="F30" s="0" t="inlineStr">
+        <is>
+          <t>Coca-Cola joins push to cut plastic waste</t>
+        </is>
+      </c>
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t>Beverage giant, which uses 120bn bottles a year, pledges to step up recycling effort</t>
+        </is>
+      </c>
+      <c r="H30" s="0" t="inlineStr">
+        <is>
+          <t>Coca-Cola has pledged to tackle a global “packaging problem” by cutting waste, as consumer giants intensify efforts to</t>
+        </is>
+      </c>
+      <c r="I30" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/9059c2dc-fd30-11e7-9b32-d7d59aace167</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="31">
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>Coca-Cola Co</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>5/7/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>5/4/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>5/10/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="32">
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t>5/18/2018 5:48:34 PM</t>
+        </is>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>Campbell Soup woes knock wider packaged food stocks</t>
+        </is>
+      </c>
+      <c r="H32" s="0" t="inlineStr">
+        <is>
+          <t>Campbell Soup is on track for its worst one-day drop in over 19 years on Friday following a profit warning and the</t>
+        </is>
+      </c>
+      <c r="I32" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/853d618e-5ab8-11e8-b8b2-d6ceb45fa9d0</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>6/12/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>6/9/2017 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>6/15/2017 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="34">
+      <c r="E34" s="0" t="inlineStr">
+        <is>
+          <t>6/14/2017 12:50:44 AM</t>
+        </is>
+      </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>Apple raises $1bn through ‘green bond’ in environmental push</t>
+        </is>
+      </c>
+      <c r="G34" s="0" t="inlineStr">
+        <is>
+          <t>10-year issue comes weeks after Donald Trump withdraws US from Paris climate agreement</t>
+        </is>
+      </c>
+      <c r="H34" s="0" t="inlineStr">
+        <is>
+          <t>Apple has raised $1bn in debt in a “green bond” to fund environmentally focused initiatives, weeks after the company’s</t>
+        </is>
+      </c>
+      <c r="I34" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/db5b911e-508a-11e7-bfb8-997009366969</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="35">
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t>6/13/2017 11:35:29 PM</t>
+        </is>
+      </c>
+      <c r="F35" s="0" t="inlineStr">
+        <is>
+          <t>AOL chief predicts lift in digital ad prices</t>
+        </is>
+      </c>
+      <c r="G35" s="0" t="inlineStr">
+        <is>
+          <t>Tim Armstrong ’bullish’ as Verizon faces Google and Facebook after Yahoo merger</t>
+        </is>
+      </c>
+      <c r="H35" s="0" t="inlineStr">
+        <is>
+          <t>Digital advertising will get “a lot more expensive” in the future as consumers’ adoption of ad blocking limits supply,</t>
+        </is>
+      </c>
+      <c r="I35" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/36a245ac-5083-11e7-bfb8-997009366969</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="36">
+      <c r="E36" s="0" t="inlineStr">
+        <is>
+          <t>6/12/2017 9:35:49 PM</t>
+        </is>
+      </c>
+      <c r="F36" s="0" t="inlineStr">
+        <is>
+          <t>US tech stocks extend losses despite late recovery</t>
+        </is>
+      </c>
+      <c r="G36" s="0" t="inlineStr">
+        <is>
+          <t>Sector that is leading gains for year pulls back on concerns of stretched valuations</t>
+        </is>
+      </c>
+      <c r="H36" s="0" t="inlineStr">
+        <is>
+          <t>US technology stocks were under further pressure on Monday despite a late recovery from the day’s lows, with investors</t>
+        </is>
+      </c>
+      <c r="I36" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/06e6ce4c-4f42-11e7-bfb8-997009366969</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="37">
+      <c r="E37" s="0" t="inlineStr">
+        <is>
+          <t>6/12/2017 10:23:40 AM</t>
+        </is>
+      </c>
+      <c r="F37" s="0" t="inlineStr">
+        <is>
+          <t>Virtual reality or augmented reality? Here’s a guide</t>
+        </is>
+      </c>
+      <c r="G37" s="0" t="inlineStr">
+        <is>
+          <t>Apple’s ARkit promises to make it easier for app makers to develop the technology</t>
+        </is>
+      </c>
+      <c r="H37" s="0" t="inlineStr">
+        <is>
+          <t>The IT crowd is addicted to acronyms. Most people can live a long and happy life without ever needing to know the</t>
+        </is>
+      </c>
+      <c r="I37" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/cba1b33c-4c6d-11e7-a3f4-c742b9791d43</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="38">
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t>6/9/2017 9:25:00 PM</t>
+        </is>
+      </c>
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>Apple shares slam into reverse in tech stock sell-off</t>
+        </is>
+      </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>World’s largest company loses almost 4% in value as traders rethink rally</t>
+        </is>
+      </c>
+      <c r="H38" s="0" t="inlineStr">
+        <is>
+          <t>Apple shares suffered in a sharp sell-off that swept through technology shares on Friday, marking a violent reversal of</t>
+        </is>
+      </c>
+      <c r="I38" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/8355fdec-4d51-11e7-919a-1e14ce4af89b</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>2/5/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>2/2/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>2/8/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="40">
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t>2/7/2018 5:37:07 AM</t>
+        </is>
+      </c>
+      <c r="F40" s="0" t="inlineStr">
+        <is>
+          <t>Apple to accept Alipay payments at stores in China</t>
+        </is>
+      </c>
+      <c r="H40" s="0" t="inlineStr">
+        <is>
+          <t>Apple is opening up payment at its 41 mainland China stores to shoppers using Alipay – the first time the US tech</t>
+        </is>
+      </c>
+      <c r="I40" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/b738c326-0bc7-11e8-8eb7-42f857ea9f09</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="41">
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t>2/6/2018 6:27:39 PM</t>
+        </is>
+      </c>
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t>EU to probe Apple’s $400m deal for Shazam</t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>Acquisition of music recognition app to be investigated over competition concerns</t>
+        </is>
+      </c>
+      <c r="H41" s="0" t="inlineStr">
+        <is>
+          <t>Brussels is to investigate Apple’s purchase of Shazam, after seven countries requested that the European watchdog</t>
+        </is>
+      </c>
+      <c r="I41" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/dd899c8a-0b63-11e8-8eb7-42f857ea9f09</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="42">
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t>2/6/2018 12:24:43 PM</t>
+        </is>
+      </c>
+      <c r="F42" s="0" t="inlineStr">
+        <is>
+          <t>Apple supplier AMS bucks downbeat market trend with 10% jump</t>
+        </is>
+      </c>
+      <c r="G42" s="0" t="inlineStr">
+        <is>
+          <t>Company announced sharp rise in profits and series of new contracts</t>
+        </is>
+      </c>
+      <c r="H42" s="0" t="inlineStr">
+        <is>
+          <t>A ten per cent daily rise in the share price of a €7bn company is a decent jump on a normal day. Given the carnage</t>
+        </is>
+      </c>
+      <c r="I42" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/26a1e512-0b32-11e8-839d-41ca06376bf2</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="43">
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t>2/6/2018 2:50:18 AM</t>
+        </is>
+      </c>
+      <c r="F43" s="0" t="inlineStr">
+        <is>
+          <t>Emerging market stocks sink as equity sell-off spreads through Asia</t>
+        </is>
+      </c>
+      <c r="H43" s="0" t="inlineStr">
+        <is>
+          <t>Stocks in Asia’s emerging markets sunk on Tuesday as the rout in global equities spread across the region sending most</t>
+        </is>
+      </c>
+      <c r="I43" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/461190d2-0add-11e8-8eb7-42f857ea9f09</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="44">
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>2/5/2018 4:46:25 PM</t>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t>Content kings bet that scale is key to survival</t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="inlineStr">
+        <is>
+          <t>A Viacom-CBS reunion would be just the latest flight to scale</t>
+        </is>
+      </c>
+      <c r="H44" s="0" t="inlineStr">
+        <is>
+          <t>When in doubt, be big. That is the motto of the media industry today. There is, without question, lots of doubt around,</t>
+        </is>
+      </c>
+      <c r="I44" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/d4c0f2ec-0820-11e8-9650-9c0ad2d7c5b5</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>Intel Corporation</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>5/28/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>5/25/2018 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>5/31/2018 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>Intel Corporation</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>4/15/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>4/12/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>4/18/2019 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="47">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>Pfizer Inc.</t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>7/1/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>6/28/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>7/4/2019 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="48">
+      <c r="E48" s="0" t="inlineStr">
+        <is>
+          <t>6/27/2019 10:26:09 PM</t>
+        </is>
+      </c>
+      <c r="F48" s="0" t="inlineStr">
+        <is>
+          <t>Ex-FDA boss joins Pfizer 83 days after leaving US drug regulator</t>
+        </is>
+      </c>
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t>Move by Scott Gottlieb adds to sense of ‘revolving door’ between government and industry</t>
+        </is>
+      </c>
+      <c r="H48" s="0" t="inlineStr">
+        <is>
+          <t>Scott Gottlieb, the former chief of the US Food and Drug Administration, has joined Pfizer’s board of directors with</t>
+        </is>
+      </c>
+      <c r="I48" s="0" t="inlineStr">
+        <is>
+          <t>https://www.ft.com/content/b41af990-9922-11e9-8cfb-30c211dcd229</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="49">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>Pfizer Inc.</t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>8/19/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>8/16/2019 12:00:00 AM</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>8/22/2019 12:00:00 AM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>